<commit_message>
UsedRange bug fixed & more + data & stats
- UsedRange bug fixed
- Swapping is exact for ranges smaller than 30 cells
</commit_message>
<xml_diff>
--- a/PLDI-2012/Performance_Eval.xlsx
+++ b/PLDI-2012/Performance_Eval.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="200">
   <si>
     <t>Benchmark:</t>
   </si>
@@ -277,13 +277,352 @@
   </si>
   <si>
     <t>2.89E-050.1673775</t>
+  </si>
+  <si>
+    <t>0.02947880.4133616</t>
+  </si>
+  <si>
+    <t>Re-ran grades benchmark</t>
+  </si>
+  <si>
+    <t>Random sampling only in ranges of size &gt;= 31</t>
+  </si>
+  <si>
+    <t>Wrong nubers of formulas and inputs (cumulative):</t>
+  </si>
+  <si>
+    <t>6.44E-050.1375294</t>
+  </si>
+  <si>
+    <t>3.31E-050.8480777</t>
+  </si>
+  <si>
+    <t>2.22E-050.7727732</t>
+  </si>
+  <si>
+    <t>3.73E-050.4319171</t>
+  </si>
+  <si>
+    <t>0.00033361.2325116</t>
+  </si>
+  <si>
+    <t>0.00034871.0926518</t>
+  </si>
+  <si>
+    <t>4.21E-050.1435117</t>
+  </si>
+  <si>
+    <t>8.79E-050.0605473</t>
+  </si>
+  <si>
+    <t>0.00036860.1221746</t>
+  </si>
+  <si>
+    <t>0.03177010.3929328</t>
+  </si>
+  <si>
+    <t>4.57E-050.1173409</t>
+  </si>
+  <si>
+    <t>4.21E-050.224006</t>
+  </si>
+  <si>
+    <t>2.4E-050.3428968</t>
+  </si>
+  <si>
+    <t>0.00081859.5679214</t>
+  </si>
+  <si>
+    <t>6E-070.7257892</t>
+  </si>
+  <si>
+    <t>Has formulas, but output says 0 formulas</t>
+  </si>
+  <si>
+    <t>Also changed the formula cells identification -- it is now done on a one-by-one basis rather than using the SpecialCells method</t>
+  </si>
+  <si>
+    <t>3.85E-050.136718</t>
+  </si>
+  <si>
+    <t>2.89E-050.8244596</t>
+  </si>
+  <si>
+    <t>2.22E-050.6652359</t>
+  </si>
+  <si>
+    <t>4.09E-050.4280399</t>
+  </si>
+  <si>
+    <t>0.00031621.2541125</t>
+  </si>
+  <si>
+    <t>0.0003831.0843666</t>
+  </si>
+  <si>
+    <t>4.33E-050.1396658</t>
+  </si>
+  <si>
+    <t>8.91E-050.0761207</t>
+  </si>
+  <si>
+    <t>may be a good visual</t>
+  </si>
+  <si>
+    <t>0.00035590.1214693</t>
+  </si>
+  <si>
+    <t>0.03054320.4034525</t>
+  </si>
+  <si>
+    <t>4.75E-050.1103978</t>
+  </si>
+  <si>
+    <t>3.91E-050.2345276</t>
+  </si>
+  <si>
+    <t>2.65E-050.333507</t>
+  </si>
+  <si>
+    <t>0.00087639.2275508</t>
+  </si>
+  <si>
+    <t>9E-060.7108049</t>
+  </si>
+  <si>
+    <t>8.13E-052.5130727</t>
+  </si>
+  <si>
+    <t>7.46E-051.2384133</t>
+  </si>
+  <si>
+    <t>0.001346266.6598829</t>
+  </si>
+  <si>
+    <t>9.21E-050.429162</t>
+  </si>
+  <si>
+    <t>0.00038428.871252</t>
+  </si>
+  <si>
+    <t>4.15E-051.007687</t>
+  </si>
+  <si>
+    <t>0.00108783.2204739</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time.xls </t>
+  </si>
+  <si>
+    <t>Still can't figure out why I'm getting an index out of bounds.</t>
+  </si>
+  <si>
+    <t>4.99E-050.498745</t>
+  </si>
+  <si>
+    <t>1.32E-050.0232411</t>
+  </si>
+  <si>
+    <t>2.16E-050.1566354</t>
+  </si>
+  <si>
+    <t>csDept-PayrollTimecardEntry.xls</t>
+  </si>
+  <si>
+    <t>5.36E-050.5454705</t>
+  </si>
+  <si>
+    <t>Form5.xls</t>
+  </si>
+  <si>
+    <t>1.2E-0569.2414527</t>
+  </si>
+  <si>
+    <t>pfi-anxa.xls</t>
+  </si>
+  <si>
+    <t>7.83E-0512.3487225</t>
+  </si>
+  <si>
+    <t>ReqComp.xls</t>
+  </si>
+  <si>
+    <t>1.8E-050.2355136</t>
+  </si>
+  <si>
+    <t>3660%20schedule%20S2003.xls</t>
+  </si>
+  <si>
+    <t>1.2E-060.1837688</t>
+  </si>
+  <si>
+    <t>Inventory%20errors.xls</t>
+  </si>
+  <si>
+    <t>3.97E-050.2710002</t>
+  </si>
+  <si>
+    <t>am_skandia_fin_supple#A80EE.xls</t>
+  </si>
+  <si>
+    <t>6.68E-050.4885788</t>
+  </si>
+  <si>
+    <t>found outliers, may be good visual</t>
+  </si>
+  <si>
+    <t>Grades_EEE481&amp;581.xls</t>
+  </si>
+  <si>
+    <t>0.00042820.6711297</t>
+  </si>
+  <si>
+    <t>Raw input count:</t>
+  </si>
+  <si>
+    <t>Inputs to computations:</t>
+  </si>
+  <si>
+    <t>0.00040890.5019795</t>
+  </si>
+  <si>
+    <t>7.28E-050.4937125</t>
+  </si>
+  <si>
+    <t>3.97E-050.2629157</t>
+  </si>
+  <si>
+    <t>1.2E-060.1759812</t>
+  </si>
+  <si>
+    <t>7.52E-0511.7593568</t>
+  </si>
+  <si>
+    <t>1.68E-050.230395</t>
+  </si>
+  <si>
+    <t>5.05E-050.551418</t>
+  </si>
+  <si>
+    <t>4.69E-050.4882083</t>
+  </si>
+  <si>
+    <t>Changed the way of counting inputs to computations: ONLY COUNT CELLS THAT ARE EVER SWAPPED, count it each time it is involved in swapping</t>
+  </si>
+  <si>
+    <t>0.00036560.5088901</t>
+  </si>
+  <si>
+    <t>6.68E-050.4929373</t>
+  </si>
+  <si>
+    <t>4.09E-050.2760478</t>
+  </si>
+  <si>
+    <t>1.8E-060.1842182</t>
+  </si>
+  <si>
+    <t>0.000104212.1389153</t>
+  </si>
+  <si>
+    <t>0.00038660.92444</t>
+  </si>
+  <si>
+    <t>Fixed used range bug</t>
+  </si>
+  <si>
+    <t>7.89E-050.9838369</t>
+  </si>
+  <si>
+    <t>3.97E-050.5369517</t>
+  </si>
+  <si>
+    <t>1.2E-060.3365235</t>
+  </si>
+  <si>
+    <t>7.89E-0523.8403775</t>
+  </si>
+  <si>
+    <t>1.74E-050.4566351</t>
+  </si>
+  <si>
+    <t>4.81E-051.0620652</t>
+  </si>
+  <si>
+    <t>5.11E-050.9724082</t>
+  </si>
+  <si>
+    <t>0.0010956.0129821</t>
+  </si>
+  <si>
+    <t>4.03E-051.9151899</t>
+  </si>
+  <si>
+    <t>0.000349915.447223</t>
+  </si>
+  <si>
+    <t>0.00012880.9462253</t>
+  </si>
+  <si>
+    <t>0.0012245125.4799425</t>
+  </si>
+  <si>
+    <t>6.98E-052.5958679</t>
+  </si>
+  <si>
+    <t>0.00010114.7414102</t>
+  </si>
+  <si>
+    <t>8.4E-061.4589523</t>
+  </si>
+  <si>
+    <t>2.59E-050.6279531</t>
+  </si>
+  <si>
+    <t>4.27E-050.4806352</t>
+  </si>
+  <si>
+    <t>4.93E-050.2133098</t>
+  </si>
+  <si>
+    <t>0.02889280.7204465</t>
+  </si>
+  <si>
+    <t>0.00033610.2361557</t>
+  </si>
+  <si>
+    <t>9.21E-050.1221861</t>
+  </si>
+  <si>
+    <t>4.63E-050.2732156</t>
+  </si>
+  <si>
+    <t>0.00036921.8897925</t>
+  </si>
+  <si>
+    <t>0.00030652.201507</t>
+  </si>
+  <si>
+    <t>4.27E-050.8415581</t>
+  </si>
+  <si>
+    <t>2.46E-051.2678307</t>
+  </si>
+  <si>
+    <t>2.95E-051.5465439</t>
+  </si>
+  <si>
+    <t>3.67E-050.2502305</t>
+  </si>
+  <si>
+    <t>0.000897414.1441081</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,13 +630,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -312,9 +665,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,10 +972,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <pane ySplit="5100" topLeftCell="A154" activePane="bottomLeft"/>
+      <selection activeCell="A92" sqref="A92"/>
+      <selection pane="bottomLeft" activeCell="A137" sqref="A137:J167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,6 +1819,11 @@
         <v>21</v>
       </c>
     </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
@@ -2085,8 +2448,3034 @@
         <v>21</v>
       </c>
     </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55" t="s">
+        <v>4</v>
+      </c>
+      <c r="E55" t="s">
+        <v>5</v>
+      </c>
+      <c r="F55" t="s">
+        <v>6</v>
+      </c>
+      <c r="G55" t="s">
+        <v>7</v>
+      </c>
+      <c r="H55" t="s">
+        <v>8</v>
+      </c>
+      <c r="I55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>34</v>
+      </c>
+      <c r="B56">
+        <v>227</v>
+      </c>
+      <c r="C56">
+        <v>483896</v>
+      </c>
+      <c r="D56">
+        <v>177.36773439999999</v>
+      </c>
+      <c r="E56">
+        <v>1.7528094000000001</v>
+      </c>
+      <c r="F56">
+        <v>174.51874190000001</v>
+      </c>
+      <c r="G56" t="s">
+        <v>87</v>
+      </c>
+      <c r="H56">
+        <v>1.03535E-2</v>
+      </c>
+      <c r="I56">
+        <v>0.64298920000000004</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
+        <v>2</v>
+      </c>
+      <c r="D60" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" t="s">
+        <v>6</v>
+      </c>
+      <c r="G60" t="s">
+        <v>7</v>
+      </c>
+      <c r="H60" t="s">
+        <v>8</v>
+      </c>
+      <c r="I60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61">
+        <v>125</v>
+      </c>
+      <c r="C61">
+        <v>421</v>
+      </c>
+      <c r="D61">
+        <v>2.3873091999999998</v>
+      </c>
+      <c r="E61">
+        <v>1.0386711</v>
+      </c>
+      <c r="F61">
+        <v>1.2110082</v>
+      </c>
+      <c r="G61" t="s">
+        <v>91</v>
+      </c>
+      <c r="H61" s="1">
+        <v>3.43E-5</v>
+      </c>
+      <c r="I61" s="1">
+        <v>1.7999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62">
+        <v>22</v>
+      </c>
+      <c r="C62">
+        <v>148</v>
+      </c>
+      <c r="D62">
+        <v>3.8373716999999998</v>
+      </c>
+      <c r="E62">
+        <v>0.27312409999999998</v>
+      </c>
+      <c r="F62">
+        <v>2.7161031000000002</v>
+      </c>
+      <c r="G62" t="s">
+        <v>92</v>
+      </c>
+      <c r="H62" s="1">
+        <v>3.2499999999999997E-5</v>
+      </c>
+      <c r="I62" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>17</v>
+      </c>
+      <c r="B63">
+        <v>3</v>
+      </c>
+      <c r="C63">
+        <v>39</v>
+      </c>
+      <c r="D63">
+        <v>2.3186651999999999</v>
+      </c>
+      <c r="E63">
+        <v>0.26911970000000002</v>
+      </c>
+      <c r="F63">
+        <v>1.2277651999999999</v>
+      </c>
+      <c r="G63" t="s">
+        <v>93</v>
+      </c>
+      <c r="H63" s="1">
+        <v>2.65E-5</v>
+      </c>
+      <c r="I63">
+        <v>4.8958399999999999E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64">
+        <v>42</v>
+      </c>
+      <c r="C64">
+        <v>120</v>
+      </c>
+      <c r="D64">
+        <v>3.5178918000000001</v>
+      </c>
+      <c r="E64">
+        <v>0.5249315</v>
+      </c>
+      <c r="F64">
+        <v>2.5259537000000001</v>
+      </c>
+      <c r="G64" t="s">
+        <v>94</v>
+      </c>
+      <c r="H64" s="1">
+        <v>3.3699999999999999E-5</v>
+      </c>
+      <c r="I64">
+        <v>3.5018500000000001E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>22</v>
+      </c>
+      <c r="B65">
+        <v>42</v>
+      </c>
+      <c r="C65">
+        <v>2100</v>
+      </c>
+      <c r="D65">
+        <v>37.637781099999998</v>
+      </c>
+      <c r="E65">
+        <v>1.6934233999999999</v>
+      </c>
+      <c r="F65">
+        <v>34.676521200000003</v>
+      </c>
+      <c r="G65" t="s">
+        <v>95</v>
+      </c>
+      <c r="H65" s="1">
+        <v>7.1000000000000005E-5</v>
+      </c>
+      <c r="I65">
+        <v>3.4920300000000001E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>25</v>
+      </c>
+      <c r="B66">
+        <v>93</v>
+      </c>
+      <c r="C66">
+        <v>2192</v>
+      </c>
+      <c r="D66">
+        <v>60.039042500000001</v>
+      </c>
+      <c r="E66">
+        <v>1.775971</v>
+      </c>
+      <c r="F66">
+        <v>57.118845499999999</v>
+      </c>
+      <c r="G66" t="s">
+        <v>96</v>
+      </c>
+      <c r="H66" s="1">
+        <v>8.7299999999999994E-5</v>
+      </c>
+      <c r="I66">
+        <v>5.1138200000000002E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>28</v>
+      </c>
+      <c r="B67">
+        <v>71</v>
+      </c>
+      <c r="C67">
+        <v>175</v>
+      </c>
+      <c r="D67">
+        <v>2.4842995999999999</v>
+      </c>
+      <c r="E67">
+        <v>0.79484699999999997</v>
+      </c>
+      <c r="F67">
+        <v>1.5302863</v>
+      </c>
+      <c r="G67" t="s">
+        <v>97</v>
+      </c>
+      <c r="H67" s="1">
+        <v>3.2499999999999997E-5</v>
+      </c>
+      <c r="I67">
+        <v>1.558E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68">
+        <v>57</v>
+      </c>
+      <c r="C68">
+        <v>396</v>
+      </c>
+      <c r="D68">
+        <v>3.0681333999999998</v>
+      </c>
+      <c r="E68">
+        <v>0.74762510000000004</v>
+      </c>
+      <c r="F68">
+        <v>2.2437162000000002</v>
+      </c>
+      <c r="G68" t="s">
+        <v>98</v>
+      </c>
+      <c r="H68" s="1">
+        <v>3.9100000000000002E-5</v>
+      </c>
+      <c r="I68">
+        <v>1.6117800000000002E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>32</v>
+      </c>
+      <c r="B69">
+        <v>80</v>
+      </c>
+      <c r="C69">
+        <v>2460</v>
+      </c>
+      <c r="D69">
+        <v>124.7661076</v>
+      </c>
+      <c r="E69">
+        <v>1.4598660999999999</v>
+      </c>
+      <c r="F69">
+        <v>123.1319578</v>
+      </c>
+      <c r="G69" t="s">
+        <v>99</v>
+      </c>
+      <c r="H69" s="1">
+        <v>8.4300000000000003E-5</v>
+      </c>
+      <c r="I69">
+        <v>5.1656199999999999E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>34</v>
+      </c>
+      <c r="B70">
+        <v>227</v>
+      </c>
+      <c r="C70">
+        <v>483896</v>
+      </c>
+      <c r="D70">
+        <v>162.4800832</v>
+      </c>
+      <c r="E70">
+        <v>1.9806017</v>
+      </c>
+      <c r="F70">
+        <v>159.32072719999999</v>
+      </c>
+      <c r="G70" t="s">
+        <v>100</v>
+      </c>
+      <c r="H70">
+        <v>1.0686599999999999E-2</v>
+      </c>
+      <c r="I70">
+        <v>0.74336480000000005</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B71">
+        <v>106</v>
+      </c>
+      <c r="C71">
+        <v>168</v>
+      </c>
+      <c r="D71">
+        <v>1.4754265</v>
+      </c>
+      <c r="E71">
+        <v>0.90563450000000001</v>
+      </c>
+      <c r="F71">
+        <v>0.42883009999999999</v>
+      </c>
+      <c r="G71" t="s">
+        <v>101</v>
+      </c>
+      <c r="H71" s="1">
+        <v>3.8500000000000001E-5</v>
+      </c>
+      <c r="I71">
+        <v>2.35368E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>38</v>
+      </c>
+      <c r="B72">
+        <v>61</v>
+      </c>
+      <c r="C72">
+        <v>143</v>
+      </c>
+      <c r="D72">
+        <v>1.7961054999999999</v>
+      </c>
+      <c r="E72">
+        <v>0.5916034</v>
+      </c>
+      <c r="F72">
+        <v>0.95697449999999995</v>
+      </c>
+      <c r="G72" t="s">
+        <v>102</v>
+      </c>
+      <c r="H72" s="1">
+        <v>4.57E-5</v>
+      </c>
+      <c r="I72">
+        <v>2.3433800000000001E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>40</v>
+      </c>
+      <c r="B73">
+        <v>36</v>
+      </c>
+      <c r="C73">
+        <v>38</v>
+      </c>
+      <c r="D73">
+        <v>1.2821937999999999</v>
+      </c>
+      <c r="E73">
+        <v>0.45118819999999998</v>
+      </c>
+      <c r="F73">
+        <v>0.46489619999999998</v>
+      </c>
+      <c r="G73" t="s">
+        <v>103</v>
+      </c>
+      <c r="H73" s="1">
+        <v>2.7100000000000001E-5</v>
+      </c>
+      <c r="I73">
+        <v>2.3161500000000002E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>42</v>
+      </c>
+      <c r="B74">
+        <v>1066</v>
+      </c>
+      <c r="C74">
+        <v>6788</v>
+      </c>
+      <c r="D74">
+        <v>303.9410383</v>
+      </c>
+      <c r="E74">
+        <v>8.3869612</v>
+      </c>
+      <c r="F74">
+        <v>285.8715833</v>
+      </c>
+      <c r="G74" t="s">
+        <v>104</v>
+      </c>
+      <c r="H74">
+        <v>1.9090000000000001E-4</v>
+      </c>
+      <c r="I74">
+        <v>0.113563</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>44</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>1.8646176000000001</v>
+      </c>
+      <c r="E75">
+        <v>0.3352019</v>
+      </c>
+      <c r="F75">
+        <v>0.80359950000000002</v>
+      </c>
+      <c r="G75" t="s">
+        <v>105</v>
+      </c>
+      <c r="H75" s="1">
+        <v>2.5199999999999999E-5</v>
+      </c>
+      <c r="I75" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K77" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" t="s">
+        <v>2</v>
+      </c>
+      <c r="D78" t="s">
+        <v>4</v>
+      </c>
+      <c r="E78" t="s">
+        <v>5</v>
+      </c>
+      <c r="F78" t="s">
+        <v>6</v>
+      </c>
+      <c r="G78" t="s">
+        <v>7</v>
+      </c>
+      <c r="H78" t="s">
+        <v>8</v>
+      </c>
+      <c r="I78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79" s="3">
+        <v>3</v>
+      </c>
+      <c r="C79" s="3">
+        <v>16</v>
+      </c>
+      <c r="D79" s="3">
+        <v>0.2306936</v>
+      </c>
+      <c r="E79" s="3">
+        <v>7.93938E-2</v>
+      </c>
+      <c r="F79" s="3">
+        <v>0.110655</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H79" s="4">
+        <v>2.4000000000000001E-5</v>
+      </c>
+      <c r="I79" s="3">
+        <v>1.73665E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B80" s="3">
+        <v>41</v>
+      </c>
+      <c r="C80" s="3">
+        <v>76</v>
+      </c>
+      <c r="D80" s="3">
+        <v>1.6514283000000001</v>
+      </c>
+      <c r="E80" s="3">
+        <v>0.36119089999999998</v>
+      </c>
+      <c r="F80" s="3">
+        <v>1.1330715</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H80" s="4">
+        <v>4.1999999999999996E-6</v>
+      </c>
+      <c r="I80" s="3">
+        <v>5.0469999999999996E-4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>15</v>
+      </c>
+      <c r="B81">
+        <v>125</v>
+      </c>
+      <c r="C81">
+        <v>421</v>
+      </c>
+      <c r="D81">
+        <v>2.2741888000000001</v>
+      </c>
+      <c r="E81">
+        <v>0.97817549999999998</v>
+      </c>
+      <c r="F81">
+        <v>1.1592231</v>
+      </c>
+      <c r="G81" t="s">
+        <v>108</v>
+      </c>
+      <c r="H81" s="1">
+        <v>3.2499999999999997E-5</v>
+      </c>
+      <c r="I81" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>13</v>
+      </c>
+      <c r="B82">
+        <v>22</v>
+      </c>
+      <c r="C82">
+        <v>148</v>
+      </c>
+      <c r="D82">
+        <v>3.7352506000000001</v>
+      </c>
+      <c r="E82">
+        <v>0.37877369999999999</v>
+      </c>
+      <c r="F82">
+        <v>2.5319552999999999</v>
+      </c>
+      <c r="G82" t="s">
+        <v>109</v>
+      </c>
+      <c r="H82" s="1">
+        <v>3.1300000000000002E-5</v>
+      </c>
+      <c r="I82" s="1">
+        <v>1.7999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>17</v>
+      </c>
+      <c r="B83">
+        <v>3</v>
+      </c>
+      <c r="C83">
+        <v>39</v>
+      </c>
+      <c r="D83">
+        <v>1.9707587</v>
+      </c>
+      <c r="E83">
+        <v>0.1711029</v>
+      </c>
+      <c r="F83">
+        <v>1.1081570999999999</v>
+      </c>
+      <c r="G83" t="s">
+        <v>110</v>
+      </c>
+      <c r="H83" s="1">
+        <v>3.79E-5</v>
+      </c>
+      <c r="I83">
+        <v>2.6202699999999999E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>19</v>
+      </c>
+      <c r="B84">
+        <v>42</v>
+      </c>
+      <c r="C84">
+        <v>120</v>
+      </c>
+      <c r="D84">
+        <v>3.1947949000000002</v>
+      </c>
+      <c r="E84">
+        <v>0.37120530000000002</v>
+      </c>
+      <c r="F84">
+        <v>2.3712865999999999</v>
+      </c>
+      <c r="G84" t="s">
+        <v>111</v>
+      </c>
+      <c r="H84" s="1">
+        <v>3.9100000000000002E-5</v>
+      </c>
+      <c r="I84">
+        <v>2.4183099999999999E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>22</v>
+      </c>
+      <c r="B85">
+        <v>42</v>
+      </c>
+      <c r="C85">
+        <v>2100</v>
+      </c>
+      <c r="D85">
+        <v>37.832564400000003</v>
+      </c>
+      <c r="E85">
+        <v>1.6597991999999999</v>
+      </c>
+      <c r="F85">
+        <v>34.883317400000003</v>
+      </c>
+      <c r="G85" t="s">
+        <v>112</v>
+      </c>
+      <c r="H85" s="1">
+        <v>6.86E-5</v>
+      </c>
+      <c r="I85">
+        <v>3.4950500000000002E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>25</v>
+      </c>
+      <c r="B86">
+        <v>93</v>
+      </c>
+      <c r="C86">
+        <v>2192</v>
+      </c>
+      <c r="D86">
+        <v>60.614635700000001</v>
+      </c>
+      <c r="E86">
+        <v>1.8047054</v>
+      </c>
+      <c r="F86">
+        <v>57.681906099999999</v>
+      </c>
+      <c r="G86" t="s">
+        <v>113</v>
+      </c>
+      <c r="H86" s="1">
+        <v>7.7000000000000001E-5</v>
+      </c>
+      <c r="I86">
+        <v>4.3197600000000003E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>28</v>
+      </c>
+      <c r="B87">
+        <v>71</v>
+      </c>
+      <c r="C87">
+        <v>175</v>
+      </c>
+      <c r="D87">
+        <v>2.4366614000000002</v>
+      </c>
+      <c r="E87">
+        <v>0.81277129999999997</v>
+      </c>
+      <c r="F87">
+        <v>1.4678982</v>
+      </c>
+      <c r="G87" t="s">
+        <v>114</v>
+      </c>
+      <c r="H87" s="1">
+        <v>4.6900000000000002E-5</v>
+      </c>
+      <c r="I87">
+        <v>1.6235900000000001E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>30</v>
+      </c>
+      <c r="B88">
+        <v>57</v>
+      </c>
+      <c r="C88">
+        <v>396</v>
+      </c>
+      <c r="D88">
+        <v>2.9014783</v>
+      </c>
+      <c r="E88">
+        <v>0.61872839999999996</v>
+      </c>
+      <c r="F88">
+        <v>2.1901030000000001</v>
+      </c>
+      <c r="G88" t="s">
+        <v>115</v>
+      </c>
+      <c r="H88" s="1">
+        <v>5.4799999999999997E-5</v>
+      </c>
+      <c r="I88">
+        <v>1.6382299999999999E-2</v>
+      </c>
+      <c r="K88" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>32</v>
+      </c>
+      <c r="B89">
+        <v>80</v>
+      </c>
+      <c r="C89">
+        <v>2460</v>
+      </c>
+      <c r="D89">
+        <v>121.2198231</v>
+      </c>
+      <c r="E89">
+        <v>1.1688984</v>
+      </c>
+      <c r="F89">
+        <v>119.87443589999999</v>
+      </c>
+      <c r="G89" t="s">
+        <v>117</v>
+      </c>
+      <c r="H89" s="1">
+        <v>8.5500000000000005E-5</v>
+      </c>
+      <c r="I89">
+        <v>5.4578099999999997E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>34</v>
+      </c>
+      <c r="B90">
+        <v>227</v>
+      </c>
+      <c r="C90">
+        <v>483896</v>
+      </c>
+      <c r="D90">
+        <v>164.60913170000001</v>
+      </c>
+      <c r="E90">
+        <v>1.8898473</v>
+      </c>
+      <c r="F90">
+        <v>161.5212416</v>
+      </c>
+      <c r="G90" t="s">
+        <v>118</v>
+      </c>
+      <c r="H90">
+        <v>9.9649999999999999E-3</v>
+      </c>
+      <c r="I90">
+        <v>0.75408209999999998</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>36</v>
+      </c>
+      <c r="B91">
+        <v>106</v>
+      </c>
+      <c r="C91">
+        <v>168</v>
+      </c>
+      <c r="D91">
+        <v>1.2639176999999999</v>
+      </c>
+      <c r="E91">
+        <v>0.70315110000000003</v>
+      </c>
+      <c r="F91">
+        <v>0.42599369999999998</v>
+      </c>
+      <c r="G91" t="s">
+        <v>119</v>
+      </c>
+      <c r="H91" s="1">
+        <v>3.0700000000000001E-5</v>
+      </c>
+      <c r="I91">
+        <v>2.42969E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>38</v>
+      </c>
+      <c r="B92">
+        <v>61</v>
+      </c>
+      <c r="C92">
+        <v>143</v>
+      </c>
+      <c r="D92">
+        <v>1.7100644</v>
+      </c>
+      <c r="E92">
+        <v>0.48195969999999999</v>
+      </c>
+      <c r="F92">
+        <v>0.96909829999999997</v>
+      </c>
+      <c r="G92" t="s">
+        <v>120</v>
+      </c>
+      <c r="H92" s="1">
+        <v>2.8900000000000001E-5</v>
+      </c>
+      <c r="I92">
+        <v>2.44108E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>40</v>
+      </c>
+      <c r="B93">
+        <v>36</v>
+      </c>
+      <c r="C93">
+        <v>38</v>
+      </c>
+      <c r="D93">
+        <v>1.1080159999999999</v>
+      </c>
+      <c r="E93">
+        <v>0.28381790000000001</v>
+      </c>
+      <c r="F93">
+        <v>0.46664410000000001</v>
+      </c>
+      <c r="G93" t="s">
+        <v>121</v>
+      </c>
+      <c r="H93" s="1">
+        <v>2.7100000000000001E-5</v>
+      </c>
+      <c r="I93">
+        <v>2.3993400000000002E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>42</v>
+      </c>
+      <c r="B94">
+        <v>1066</v>
+      </c>
+      <c r="C94">
+        <v>6788</v>
+      </c>
+      <c r="D94">
+        <v>316.09232989999998</v>
+      </c>
+      <c r="E94">
+        <v>9.2284548999999991</v>
+      </c>
+      <c r="F94">
+        <v>297.51840279999999</v>
+      </c>
+      <c r="G94" t="s">
+        <v>122</v>
+      </c>
+      <c r="H94">
+        <v>2.186E-4</v>
+      </c>
+      <c r="I94">
+        <v>0.1168265</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>44</v>
+      </c>
+      <c r="B95">
+        <v>33</v>
+      </c>
+      <c r="C95">
+        <v>92</v>
+      </c>
+      <c r="D95">
+        <v>2.016794</v>
+      </c>
+      <c r="E95">
+        <v>0.48106640000000001</v>
+      </c>
+      <c r="F95">
+        <v>0.82488479999999997</v>
+      </c>
+      <c r="G95" t="s">
+        <v>123</v>
+      </c>
+      <c r="H95" s="1">
+        <v>2.7699999999999999E-5</v>
+      </c>
+      <c r="I95" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>48</v>
+      </c>
+      <c r="B96">
+        <v>72</v>
+      </c>
+      <c r="C96">
+        <v>367</v>
+      </c>
+      <c r="D96">
+        <v>8.6630219999999998</v>
+      </c>
+      <c r="E96">
+        <v>0.97879769999999999</v>
+      </c>
+      <c r="F96">
+        <v>5.1430695999999996</v>
+      </c>
+      <c r="G96" t="s">
+        <v>124</v>
+      </c>
+      <c r="H96" s="1">
+        <v>3.79E-5</v>
+      </c>
+      <c r="I96">
+        <v>2.7962799999999999E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>50</v>
+      </c>
+      <c r="B97">
+        <v>73</v>
+      </c>
+      <c r="C97">
+        <v>340</v>
+      </c>
+      <c r="D97">
+        <v>4.7783638000000002</v>
+      </c>
+      <c r="E97">
+        <v>1.6609586999999999</v>
+      </c>
+      <c r="F97">
+        <v>1.8600118000000001</v>
+      </c>
+      <c r="G97" t="s">
+        <v>125</v>
+      </c>
+      <c r="H97" s="1">
+        <v>3.7299999999999999E-5</v>
+      </c>
+      <c r="I97">
+        <v>1.8868099999999999E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>52</v>
+      </c>
+      <c r="B98">
+        <v>2626</v>
+      </c>
+      <c r="C98">
+        <v>10109</v>
+      </c>
+      <c r="D98">
+        <v>453.295591</v>
+      </c>
+      <c r="E98">
+        <v>27.997608100000001</v>
+      </c>
+      <c r="F98">
+        <v>358.55928390000003</v>
+      </c>
+      <c r="G98" t="s">
+        <v>126</v>
+      </c>
+      <c r="H98">
+        <v>2.3250000000000001E-4</v>
+      </c>
+      <c r="I98">
+        <v>7.7237399999999998E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>54</v>
+      </c>
+      <c r="B99">
+        <v>69</v>
+      </c>
+      <c r="C99">
+        <v>465</v>
+      </c>
+      <c r="D99">
+        <v>4.8037045999999997</v>
+      </c>
+      <c r="E99">
+        <v>0.79109260000000003</v>
+      </c>
+      <c r="F99">
+        <v>3.5511921000000002</v>
+      </c>
+      <c r="G99" t="s">
+        <v>127</v>
+      </c>
+      <c r="H99" s="1">
+        <v>4.2700000000000001E-5</v>
+      </c>
+      <c r="I99">
+        <v>3.2123100000000002E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>56</v>
+      </c>
+      <c r="B100">
+        <v>797</v>
+      </c>
+      <c r="C100">
+        <v>3271</v>
+      </c>
+      <c r="D100">
+        <v>77.2200852</v>
+      </c>
+      <c r="E100">
+        <v>6.7546628000000002</v>
+      </c>
+      <c r="F100">
+        <v>61.559589899999999</v>
+      </c>
+      <c r="G100" t="s">
+        <v>128</v>
+      </c>
+      <c r="H100" s="1">
+        <v>9.5699999999999995E-5</v>
+      </c>
+      <c r="I100">
+        <v>3.4100600000000002E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>58</v>
+      </c>
+      <c r="B101">
+        <v>79</v>
+      </c>
+      <c r="C101">
+        <v>497</v>
+      </c>
+      <c r="D101">
+        <v>3.4706393000000002</v>
+      </c>
+      <c r="E101">
+        <v>1.0648588000000001</v>
+      </c>
+      <c r="F101">
+        <v>1.3980147000000001</v>
+      </c>
+      <c r="G101" t="s">
+        <v>129</v>
+      </c>
+      <c r="H101" s="1">
+        <v>3.6100000000000003E-5</v>
+      </c>
+      <c r="I101" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>59</v>
+      </c>
+      <c r="B102">
+        <v>335</v>
+      </c>
+      <c r="C102">
+        <v>6945</v>
+      </c>
+      <c r="D102">
+        <v>115.0990374</v>
+      </c>
+      <c r="E102">
+        <v>4.3033878000000003</v>
+      </c>
+      <c r="F102">
+        <v>107.5114741</v>
+      </c>
+      <c r="G102" t="s">
+        <v>130</v>
+      </c>
+      <c r="H102">
+        <v>1.716E-4</v>
+      </c>
+      <c r="I102">
+        <v>6.2442200000000003E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>63</v>
+      </c>
+      <c r="B103">
+        <v>2</v>
+      </c>
+      <c r="C103">
+        <v>156</v>
+      </c>
+      <c r="D103">
+        <v>4.2680623000000004</v>
+      </c>
+      <c r="E103">
+        <v>0.23434930000000001</v>
+      </c>
+      <c r="F103">
+        <v>3.5116282999999999</v>
+      </c>
+      <c r="G103" t="s">
+        <v>133</v>
+      </c>
+      <c r="H103" s="1">
+        <v>3.1900000000000003E-5</v>
+      </c>
+      <c r="I103">
+        <v>2.3257900000000001E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>136</v>
+      </c>
+      <c r="B104">
+        <v>68</v>
+      </c>
+      <c r="C104">
+        <v>477</v>
+      </c>
+      <c r="D104">
+        <v>4.9857484999999997</v>
+      </c>
+      <c r="E104">
+        <v>0.59196300000000002</v>
+      </c>
+      <c r="F104">
+        <v>3.8482253000000002</v>
+      </c>
+      <c r="G104" t="s">
+        <v>137</v>
+      </c>
+      <c r="H104" s="1">
+        <v>3.4900000000000001E-5</v>
+      </c>
+      <c r="I104" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>142</v>
+      </c>
+      <c r="B105">
+        <v>54</v>
+      </c>
+      <c r="C105">
+        <v>162</v>
+      </c>
+      <c r="D105">
+        <v>0.97041840000000001</v>
+      </c>
+      <c r="E105">
+        <v>0.43527690000000002</v>
+      </c>
+      <c r="F105">
+        <v>0.29958099999999999</v>
+      </c>
+      <c r="G105" t="s">
+        <v>143</v>
+      </c>
+      <c r="H105" s="1">
+        <v>2.7699999999999999E-5</v>
+      </c>
+      <c r="I105" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>140</v>
+      </c>
+      <c r="B106">
+        <v>5</v>
+      </c>
+      <c r="C106">
+        <v>310</v>
+      </c>
+      <c r="D106">
+        <v>34.059889900000002</v>
+      </c>
+      <c r="E106">
+        <v>1.4595545999999999</v>
+      </c>
+      <c r="F106">
+        <v>20.224538500000001</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H106" s="1">
+        <v>3.3699999999999999E-5</v>
+      </c>
+      <c r="I106">
+        <v>2.6962300000000002E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>144</v>
+      </c>
+      <c r="B107">
+        <v>31</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+      <c r="D107">
+        <v>0.71117109999999994</v>
+      </c>
+      <c r="E107">
+        <v>0.31684879999999999</v>
+      </c>
+      <c r="F107">
+        <v>0.21052460000000001</v>
+      </c>
+      <c r="G107" t="s">
+        <v>145</v>
+      </c>
+      <c r="H107" s="1">
+        <v>2.65E-5</v>
+      </c>
+      <c r="I107" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>146</v>
+      </c>
+      <c r="B108">
+        <v>100</v>
+      </c>
+      <c r="C108">
+        <v>144</v>
+      </c>
+      <c r="D108">
+        <v>1.6653411</v>
+      </c>
+      <c r="E108">
+        <v>0.65089850000000005</v>
+      </c>
+      <c r="F108">
+        <v>0.74337439999999999</v>
+      </c>
+      <c r="G108" t="s">
+        <v>147</v>
+      </c>
+      <c r="H108" s="1">
+        <v>2.7100000000000001E-5</v>
+      </c>
+      <c r="I108" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>148</v>
+      </c>
+      <c r="B109">
+        <v>56</v>
+      </c>
+      <c r="C109">
+        <v>281</v>
+      </c>
+      <c r="D109">
+        <v>4.6207555999999999</v>
+      </c>
+      <c r="E109">
+        <v>0.60108779999999995</v>
+      </c>
+      <c r="F109">
+        <v>3.4996708000000001</v>
+      </c>
+      <c r="G109" t="s">
+        <v>149</v>
+      </c>
+      <c r="H109" s="1">
+        <v>3.9100000000000002E-5</v>
+      </c>
+      <c r="I109">
+        <v>3.1312300000000001E-2</v>
+      </c>
+      <c r="K109" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>151</v>
+      </c>
+      <c r="B110">
+        <v>177</v>
+      </c>
+      <c r="C110">
+        <v>1999</v>
+      </c>
+      <c r="D110">
+        <v>50.141697899999997</v>
+      </c>
+      <c r="E110">
+        <v>2.6999532999999998</v>
+      </c>
+      <c r="F110">
+        <v>46.719331599999997</v>
+      </c>
+      <c r="G110" t="s">
+        <v>152</v>
+      </c>
+      <c r="H110">
+        <v>1.1739999999999999E-4</v>
+      </c>
+      <c r="I110">
+        <v>5.0737699999999997E-2</v>
+      </c>
+      <c r="K110" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>131</v>
+      </c>
+      <c r="B113" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B114">
+        <v>1</v>
+      </c>
+      <c r="C114">
+        <v>16</v>
+      </c>
+      <c r="D114">
+        <v>146.27509409999999</v>
+      </c>
+      <c r="E114">
+        <v>4.5706632000000003</v>
+      </c>
+      <c r="F114">
+        <v>72.462958999999998</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H114" s="1">
+        <v>2.3999999999999999E-6</v>
+      </c>
+      <c r="I114" s="1">
+        <v>4.7999999999999998E-6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>0</v>
+      </c>
+      <c r="B117" t="s">
+        <v>1</v>
+      </c>
+      <c r="C117" t="s">
+        <v>153</v>
+      </c>
+      <c r="D117" t="s">
+        <v>154</v>
+      </c>
+      <c r="E117" t="s">
+        <v>4</v>
+      </c>
+      <c r="F117" t="s">
+        <v>5</v>
+      </c>
+      <c r="G117" t="s">
+        <v>6</v>
+      </c>
+      <c r="H117" t="s">
+        <v>7</v>
+      </c>
+      <c r="I117" t="s">
+        <v>8</v>
+      </c>
+      <c r="J117" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>151</v>
+      </c>
+      <c r="B118">
+        <v>177</v>
+      </c>
+      <c r="C118">
+        <v>757</v>
+      </c>
+      <c r="D118">
+        <v>1999</v>
+      </c>
+      <c r="E118">
+        <v>39.756452600000003</v>
+      </c>
+      <c r="F118">
+        <v>2.1450935000000002</v>
+      </c>
+      <c r="G118">
+        <v>37.072422299999999</v>
+      </c>
+      <c r="H118" t="s">
+        <v>155</v>
+      </c>
+      <c r="I118" s="1">
+        <v>7.5199999999999998E-5</v>
+      </c>
+      <c r="J118">
+        <v>3.6473199999999997E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>148</v>
+      </c>
+      <c r="B119">
+        <v>56</v>
+      </c>
+      <c r="C119">
+        <v>272</v>
+      </c>
+      <c r="D119">
+        <v>281</v>
+      </c>
+      <c r="E119">
+        <v>4.6767390000000004</v>
+      </c>
+      <c r="F119">
+        <v>0.62046250000000003</v>
+      </c>
+      <c r="G119">
+        <v>3.5204645999999999</v>
+      </c>
+      <c r="H119" t="s">
+        <v>156</v>
+      </c>
+      <c r="I119" s="1">
+        <v>3.5500000000000002E-5</v>
+      </c>
+      <c r="J119">
+        <v>4.1991100000000003E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>146</v>
+      </c>
+      <c r="B120">
+        <v>100</v>
+      </c>
+      <c r="C120">
+        <v>129</v>
+      </c>
+      <c r="D120">
+        <v>144</v>
+      </c>
+      <c r="E120">
+        <v>1.7092947999999999</v>
+      </c>
+      <c r="F120">
+        <v>0.64230500000000001</v>
+      </c>
+      <c r="G120">
+        <v>0.80400490000000002</v>
+      </c>
+      <c r="H120" t="s">
+        <v>157</v>
+      </c>
+      <c r="I120" s="1">
+        <v>2.83E-5</v>
+      </c>
+      <c r="J120" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>144</v>
+      </c>
+      <c r="B121">
+        <v>31</v>
+      </c>
+      <c r="C121">
+        <v>1</v>
+      </c>
+      <c r="D121">
+        <v>1</v>
+      </c>
+      <c r="E121">
+        <v>0.71300140000000001</v>
+      </c>
+      <c r="F121">
+        <v>0.3335533</v>
+      </c>
+      <c r="G121">
+        <v>0.20344229999999999</v>
+      </c>
+      <c r="H121" t="s">
+        <v>158</v>
+      </c>
+      <c r="I121" s="1">
+        <v>2.2200000000000001E-5</v>
+      </c>
+      <c r="J121" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>140</v>
+      </c>
+      <c r="B122">
+        <v>5</v>
+      </c>
+      <c r="C122">
+        <v>310</v>
+      </c>
+      <c r="D122">
+        <v>310</v>
+      </c>
+      <c r="E122">
+        <v>32.8866613</v>
+      </c>
+      <c r="F122">
+        <v>1.4489692000000001</v>
+      </c>
+      <c r="G122">
+        <v>19.65315</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I122" s="1">
+        <v>3.3699999999999999E-5</v>
+      </c>
+      <c r="J122">
+        <v>2.5076399999999999E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>142</v>
+      </c>
+      <c r="B123">
+        <v>54</v>
+      </c>
+      <c r="C123">
+        <v>162</v>
+      </c>
+      <c r="D123">
+        <v>162</v>
+      </c>
+      <c r="E123">
+        <v>0.97176649999999998</v>
+      </c>
+      <c r="F123">
+        <v>0.4369189</v>
+      </c>
+      <c r="G123">
+        <v>0.30440390000000001</v>
+      </c>
+      <c r="H123" t="s">
+        <v>160</v>
+      </c>
+      <c r="I123" s="1">
+        <v>3.0700000000000001E-5</v>
+      </c>
+      <c r="J123" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>136</v>
+      </c>
+      <c r="B124">
+        <v>68</v>
+      </c>
+      <c r="C124">
+        <v>204</v>
+      </c>
+      <c r="D124">
+        <v>477</v>
+      </c>
+      <c r="E124">
+        <v>4.8549543999999996</v>
+      </c>
+      <c r="F124">
+        <v>0.62317540000000005</v>
+      </c>
+      <c r="G124">
+        <v>3.680275</v>
+      </c>
+      <c r="H124" t="s">
+        <v>161</v>
+      </c>
+      <c r="I124" s="1">
+        <v>3.4900000000000001E-5</v>
+      </c>
+      <c r="J124" s="1">
+        <v>5.9999999999999997E-7</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>63</v>
+      </c>
+      <c r="B125">
+        <v>2</v>
+      </c>
+      <c r="C125">
+        <v>156</v>
+      </c>
+      <c r="D125">
+        <v>156</v>
+      </c>
+      <c r="E125">
+        <v>4.0534600000000003</v>
+      </c>
+      <c r="F125">
+        <v>0.24165690000000001</v>
+      </c>
+      <c r="G125">
+        <v>3.3004658999999998</v>
+      </c>
+      <c r="H125" t="s">
+        <v>162</v>
+      </c>
+      <c r="I125" s="1">
+        <v>2.8900000000000001E-5</v>
+      </c>
+      <c r="J125">
+        <v>2.30531E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>0</v>
+      </c>
+      <c r="B129" t="s">
+        <v>1</v>
+      </c>
+      <c r="C129" t="s">
+        <v>153</v>
+      </c>
+      <c r="D129" t="s">
+        <v>154</v>
+      </c>
+      <c r="E129" t="s">
+        <v>4</v>
+      </c>
+      <c r="F129" t="s">
+        <v>5</v>
+      </c>
+      <c r="G129" t="s">
+        <v>6</v>
+      </c>
+      <c r="H129" t="s">
+        <v>7</v>
+      </c>
+      <c r="I129" t="s">
+        <v>8</v>
+      </c>
+      <c r="J129" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>151</v>
+      </c>
+      <c r="B130">
+        <v>177</v>
+      </c>
+      <c r="C130">
+        <v>757</v>
+      </c>
+      <c r="D130">
+        <v>756</v>
+      </c>
+      <c r="E130">
+        <v>37.7562274</v>
+      </c>
+      <c r="F130">
+        <v>1.9831243000000001</v>
+      </c>
+      <c r="G130">
+        <v>35.207288200000001</v>
+      </c>
+      <c r="H130" t="s">
+        <v>164</v>
+      </c>
+      <c r="I130" s="1">
+        <v>7.0400000000000004E-5</v>
+      </c>
+      <c r="J130">
+        <v>5.6488799999999999E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>148</v>
+      </c>
+      <c r="B131">
+        <v>56</v>
+      </c>
+      <c r="C131">
+        <v>272</v>
+      </c>
+      <c r="D131">
+        <v>268</v>
+      </c>
+      <c r="E131">
+        <v>4.6462916999999999</v>
+      </c>
+      <c r="F131">
+        <v>0.58922479999999999</v>
+      </c>
+      <c r="G131">
+        <v>3.5216764999999999</v>
+      </c>
+      <c r="H131" t="s">
+        <v>165</v>
+      </c>
+      <c r="I131" s="1">
+        <v>3.3699999999999999E-5</v>
+      </c>
+      <c r="J131">
+        <v>4.2352599999999997E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>146</v>
+      </c>
+      <c r="B132">
+        <v>100</v>
+      </c>
+      <c r="C132">
+        <v>129</v>
+      </c>
+      <c r="D132">
+        <v>90</v>
+      </c>
+      <c r="E132">
+        <v>1.6670138999999999</v>
+      </c>
+      <c r="F132">
+        <v>0.66087260000000003</v>
+      </c>
+      <c r="G132">
+        <v>0.73002549999999999</v>
+      </c>
+      <c r="H132" t="s">
+        <v>166</v>
+      </c>
+      <c r="I132" s="1">
+        <v>2.5899999999999999E-5</v>
+      </c>
+      <c r="J132" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>144</v>
+      </c>
+      <c r="B133">
+        <v>31</v>
+      </c>
+      <c r="C133">
+        <v>1</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+      <c r="E133">
+        <v>0.70868940000000002</v>
+      </c>
+      <c r="F133">
+        <v>0.32426169999999999</v>
+      </c>
+      <c r="G133">
+        <v>0.20018250000000001</v>
+      </c>
+      <c r="H133" t="s">
+        <v>167</v>
+      </c>
+      <c r="I133" s="1">
+        <v>2.4000000000000001E-5</v>
+      </c>
+      <c r="J133" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>140</v>
+      </c>
+      <c r="B134">
+        <v>5</v>
+      </c>
+      <c r="C134">
+        <v>310</v>
+      </c>
+      <c r="D134">
+        <v>310</v>
+      </c>
+      <c r="E134">
+        <v>33.893097900000001</v>
+      </c>
+      <c r="F134">
+        <v>1.4449926</v>
+      </c>
+      <c r="G134">
+        <v>20.283816699999999</v>
+      </c>
+      <c r="H134" t="s">
+        <v>168</v>
+      </c>
+      <c r="I134" s="1">
+        <v>3.43E-5</v>
+      </c>
+      <c r="J134">
+        <v>2.5234800000000002E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>0</v>
+      </c>
+      <c r="B137" t="s">
+        <v>1</v>
+      </c>
+      <c r="C137" t="s">
+        <v>153</v>
+      </c>
+      <c r="D137" t="s">
+        <v>154</v>
+      </c>
+      <c r="E137" t="s">
+        <v>4</v>
+      </c>
+      <c r="F137" t="s">
+        <v>5</v>
+      </c>
+      <c r="G137" t="s">
+        <v>6</v>
+      </c>
+      <c r="H137" t="s">
+        <v>7</v>
+      </c>
+      <c r="I137" t="s">
+        <v>8</v>
+      </c>
+      <c r="J137" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>151</v>
+      </c>
+      <c r="B138">
+        <v>177</v>
+      </c>
+      <c r="C138">
+        <v>757</v>
+      </c>
+      <c r="D138">
+        <v>756</v>
+      </c>
+      <c r="E138">
+        <v>39.497394800000002</v>
+      </c>
+      <c r="F138">
+        <v>2.8247770000000001</v>
+      </c>
+      <c r="G138">
+        <v>35.709635200000001</v>
+      </c>
+      <c r="H138" t="s">
+        <v>169</v>
+      </c>
+      <c r="I138" s="1">
+        <v>7.1600000000000006E-5</v>
+      </c>
+      <c r="J138">
+        <v>3.8084399999999997E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>148</v>
+      </c>
+      <c r="B139">
+        <v>56</v>
+      </c>
+      <c r="C139">
+        <v>272</v>
+      </c>
+      <c r="D139">
+        <v>268</v>
+      </c>
+      <c r="E139">
+        <v>5.9395709999999999</v>
+      </c>
+      <c r="F139">
+        <v>0.82246399999999997</v>
+      </c>
+      <c r="G139">
+        <v>4.1073203999999999</v>
+      </c>
+      <c r="H139" t="s">
+        <v>171</v>
+      </c>
+      <c r="I139" s="1">
+        <v>3.43E-5</v>
+      </c>
+      <c r="J139">
+        <v>2.5836499999999998E-2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>146</v>
+      </c>
+      <c r="B140">
+        <v>100</v>
+      </c>
+      <c r="C140">
+        <v>129</v>
+      </c>
+      <c r="D140">
+        <v>90</v>
+      </c>
+      <c r="E140">
+        <v>2.3081201</v>
+      </c>
+      <c r="F140">
+        <v>0.75126800000000005</v>
+      </c>
+      <c r="G140">
+        <v>1.0198305999999999</v>
+      </c>
+      <c r="H140" t="s">
+        <v>172</v>
+      </c>
+      <c r="I140" s="1">
+        <v>2.8900000000000001E-5</v>
+      </c>
+      <c r="J140" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>144</v>
+      </c>
+      <c r="B141">
+        <v>31</v>
+      </c>
+      <c r="C141">
+        <v>1</v>
+      </c>
+      <c r="D141">
+        <v>0</v>
+      </c>
+      <c r="E141">
+        <v>1.1479702000000001</v>
+      </c>
+      <c r="F141">
+        <v>0.36907790000000001</v>
+      </c>
+      <c r="G141">
+        <v>0.44233810000000001</v>
+      </c>
+      <c r="H141" t="s">
+        <v>173</v>
+      </c>
+      <c r="I141" s="1">
+        <v>2.7699999999999999E-5</v>
+      </c>
+      <c r="J141" s="1">
+        <v>1.7999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>140</v>
+      </c>
+      <c r="B142">
+        <v>5</v>
+      </c>
+      <c r="C142">
+        <v>310</v>
+      </c>
+      <c r="D142">
+        <v>310</v>
+      </c>
+      <c r="E142">
+        <v>58.637764400000002</v>
+      </c>
+      <c r="F142">
+        <v>1.6850472999999999</v>
+      </c>
+      <c r="G142">
+        <v>33.087603000000001</v>
+      </c>
+      <c r="H142" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I142" s="1">
+        <v>3.1900000000000003E-5</v>
+      </c>
+      <c r="J142">
+        <v>2.46258E-2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>142</v>
+      </c>
+      <c r="B143">
+        <v>54</v>
+      </c>
+      <c r="C143">
+        <v>162</v>
+      </c>
+      <c r="D143">
+        <v>0</v>
+      </c>
+      <c r="E143">
+        <v>1.4969383999999999</v>
+      </c>
+      <c r="F143">
+        <v>0.50984119999999999</v>
+      </c>
+      <c r="G143">
+        <v>0.53041579999999999</v>
+      </c>
+      <c r="H143" t="s">
+        <v>175</v>
+      </c>
+      <c r="I143" s="1">
+        <v>2.7699999999999999E-5</v>
+      </c>
+      <c r="J143" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>136</v>
+      </c>
+      <c r="B144">
+        <v>68</v>
+      </c>
+      <c r="C144">
+        <v>204</v>
+      </c>
+      <c r="D144">
+        <v>124</v>
+      </c>
+      <c r="E144">
+        <v>5.8716090000000003</v>
+      </c>
+      <c r="F144">
+        <v>0.78702989999999995</v>
+      </c>
+      <c r="G144">
+        <v>4.0224302999999999</v>
+      </c>
+      <c r="H144" t="s">
+        <v>176</v>
+      </c>
+      <c r="I144" s="1">
+        <v>3.43E-5</v>
+      </c>
+      <c r="J144" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>63</v>
+      </c>
+      <c r="B145">
+        <v>2</v>
+      </c>
+      <c r="C145">
+        <v>156</v>
+      </c>
+      <c r="D145">
+        <v>156</v>
+      </c>
+      <c r="E145">
+        <v>5.0753224000000001</v>
+      </c>
+      <c r="F145">
+        <v>0.3034944</v>
+      </c>
+      <c r="G145">
+        <v>3.7759944999999999</v>
+      </c>
+      <c r="H145" t="s">
+        <v>177</v>
+      </c>
+      <c r="I145" s="1">
+        <v>2.9499999999999999E-5</v>
+      </c>
+      <c r="J145">
+        <v>2.3344699999999999E-2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>59</v>
+      </c>
+      <c r="B146">
+        <v>335</v>
+      </c>
+      <c r="C146">
+        <v>1369</v>
+      </c>
+      <c r="D146">
+        <v>1247</v>
+      </c>
+      <c r="E146">
+        <v>120.8895694</v>
+      </c>
+      <c r="F146">
+        <v>5.3495458999999999</v>
+      </c>
+      <c r="G146">
+        <v>109.45605930000001</v>
+      </c>
+      <c r="H146" t="s">
+        <v>178</v>
+      </c>
+      <c r="I146">
+        <v>1.6259999999999999E-4</v>
+      </c>
+      <c r="J146">
+        <v>6.9724499999999995E-2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>58</v>
+      </c>
+      <c r="B147">
+        <v>79</v>
+      </c>
+      <c r="C147">
+        <v>54</v>
+      </c>
+      <c r="D147">
+        <v>11</v>
+      </c>
+      <c r="E147">
+        <v>5.5596499000000001</v>
+      </c>
+      <c r="F147">
+        <v>1.2759478</v>
+      </c>
+      <c r="G147">
+        <v>2.3684346000000001</v>
+      </c>
+      <c r="H147" t="s">
+        <v>179</v>
+      </c>
+      <c r="I147" s="1">
+        <v>3.6100000000000003E-5</v>
+      </c>
+      <c r="J147" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>56</v>
+      </c>
+      <c r="B148">
+        <v>797</v>
+      </c>
+      <c r="C148">
+        <v>1160</v>
+      </c>
+      <c r="D148">
+        <v>365</v>
+      </c>
+      <c r="E148">
+        <v>91.103057500000006</v>
+      </c>
+      <c r="F148">
+        <v>8.0197866999999992</v>
+      </c>
+      <c r="G148">
+        <v>67.587009399999999</v>
+      </c>
+      <c r="H148" t="s">
+        <v>180</v>
+      </c>
+      <c r="I148" s="1">
+        <v>9.09E-5</v>
+      </c>
+      <c r="J148">
+        <v>4.8597599999999998E-2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>54</v>
+      </c>
+      <c r="B149">
+        <v>69</v>
+      </c>
+      <c r="C149">
+        <v>271</v>
+      </c>
+      <c r="D149">
+        <v>242</v>
+      </c>
+      <c r="E149">
+        <v>5.9966296999999997</v>
+      </c>
+      <c r="F149">
+        <v>1.0156354000000001</v>
+      </c>
+      <c r="G149">
+        <v>4.0188838000000002</v>
+      </c>
+      <c r="H149" t="s">
+        <v>181</v>
+      </c>
+      <c r="I149" s="1">
+        <v>3.6100000000000003E-5</v>
+      </c>
+      <c r="J149">
+        <v>1.57203E-2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>52</v>
+      </c>
+      <c r="B150">
+        <v>2626</v>
+      </c>
+      <c r="C150">
+        <v>2574</v>
+      </c>
+      <c r="D150">
+        <v>2403</v>
+      </c>
+      <c r="E150">
+        <v>562.92425300000002</v>
+      </c>
+      <c r="F150">
+        <v>32.536183700000002</v>
+      </c>
+      <c r="G150">
+        <v>404.83416679999999</v>
+      </c>
+      <c r="H150" t="s">
+        <v>182</v>
+      </c>
+      <c r="I150">
+        <v>2.186E-4</v>
+      </c>
+      <c r="J150">
+        <v>7.2516899999999995E-2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>50</v>
+      </c>
+      <c r="B151">
+        <v>73</v>
+      </c>
+      <c r="C151">
+        <v>29</v>
+      </c>
+      <c r="D151">
+        <v>26</v>
+      </c>
+      <c r="E151">
+        <v>7.5540444999999998</v>
+      </c>
+      <c r="F151">
+        <v>1.7600007</v>
+      </c>
+      <c r="G151">
+        <v>3.1782111</v>
+      </c>
+      <c r="H151" t="s">
+        <v>183</v>
+      </c>
+      <c r="I151" s="1">
+        <v>4.2700000000000001E-5</v>
+      </c>
+      <c r="J151">
+        <v>1.98523E-2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>48</v>
+      </c>
+      <c r="B152">
+        <v>72</v>
+      </c>
+      <c r="C152">
+        <v>148</v>
+      </c>
+      <c r="D152">
+        <v>142</v>
+      </c>
+      <c r="E152">
+        <v>13.380172</v>
+      </c>
+      <c r="F152">
+        <v>1.0932788</v>
+      </c>
+      <c r="G152">
+        <v>7.5128167000000001</v>
+      </c>
+      <c r="H152" t="s">
+        <v>184</v>
+      </c>
+      <c r="I152" s="1">
+        <v>3.6100000000000003E-5</v>
+      </c>
+      <c r="J152">
+        <v>3.2529099999999998E-2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>44</v>
+      </c>
+      <c r="B153">
+        <v>33</v>
+      </c>
+      <c r="C153">
+        <v>21</v>
+      </c>
+      <c r="D153">
+        <v>0</v>
+      </c>
+      <c r="E153">
+        <v>3.5766599000000001</v>
+      </c>
+      <c r="F153">
+        <v>0.51494180000000001</v>
+      </c>
+      <c r="G153">
+        <v>1.6027290999999999</v>
+      </c>
+      <c r="H153" t="s">
+        <v>185</v>
+      </c>
+      <c r="I153" s="1">
+        <v>2.65E-5</v>
+      </c>
+      <c r="J153" s="1">
+        <v>1.7999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>42</v>
+      </c>
+      <c r="B154">
+        <v>1066</v>
+      </c>
+      <c r="C154">
+        <v>3158</v>
+      </c>
+      <c r="D154">
+        <v>239</v>
+      </c>
+      <c r="E154">
+        <v>314.31300199999998</v>
+      </c>
+      <c r="F154">
+        <v>10.835630500000001</v>
+      </c>
+      <c r="G154">
+        <v>289.23876560000002</v>
+      </c>
+      <c r="H154" t="s">
+        <v>199</v>
+      </c>
+      <c r="I154">
+        <v>2.084E-4</v>
+      </c>
+      <c r="J154">
+        <v>9.3392000000000003E-2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>40</v>
+      </c>
+      <c r="B155">
+        <v>36</v>
+      </c>
+      <c r="C155">
+        <v>41</v>
+      </c>
+      <c r="D155">
+        <v>27</v>
+      </c>
+      <c r="E155">
+        <v>1.7653684999999999</v>
+      </c>
+      <c r="F155">
+        <v>0.28885339999999998</v>
+      </c>
+      <c r="G155">
+        <v>0.82435420000000004</v>
+      </c>
+      <c r="H155" t="s">
+        <v>186</v>
+      </c>
+      <c r="I155" s="1">
+        <v>2.5899999999999999E-5</v>
+      </c>
+      <c r="J155">
+        <v>2.4156E-2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>38</v>
+      </c>
+      <c r="B156">
+        <v>61</v>
+      </c>
+      <c r="C156">
+        <v>143</v>
+      </c>
+      <c r="D156">
+        <v>123</v>
+      </c>
+      <c r="E156">
+        <v>2.2048594000000001</v>
+      </c>
+      <c r="F156">
+        <v>0.56791720000000001</v>
+      </c>
+      <c r="G156">
+        <v>1.131359</v>
+      </c>
+      <c r="H156" t="s">
+        <v>187</v>
+      </c>
+      <c r="I156" s="1">
+        <v>2.8900000000000001E-5</v>
+      </c>
+      <c r="J156">
+        <v>2.48764E-2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>36</v>
+      </c>
+      <c r="B157">
+        <v>106</v>
+      </c>
+      <c r="C157">
+        <v>168</v>
+      </c>
+      <c r="D157">
+        <v>168</v>
+      </c>
+      <c r="E157">
+        <v>1.6736275</v>
+      </c>
+      <c r="F157">
+        <v>0.89180009999999998</v>
+      </c>
+      <c r="G157">
+        <v>0.53624340000000004</v>
+      </c>
+      <c r="H157" t="s">
+        <v>188</v>
+      </c>
+      <c r="I157" s="1">
+        <v>2.9499999999999999E-5</v>
+      </c>
+      <c r="J157">
+        <v>3.2195399999999999E-2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>34</v>
+      </c>
+      <c r="B158">
+        <v>227</v>
+      </c>
+      <c r="C158">
+        <v>661</v>
+      </c>
+      <c r="D158">
+        <v>96</v>
+      </c>
+      <c r="E158">
+        <v>154.98085810000001</v>
+      </c>
+      <c r="F158">
+        <v>2.4295727999999999</v>
+      </c>
+      <c r="G158">
+        <v>150.99316039999999</v>
+      </c>
+      <c r="H158" t="s">
+        <v>189</v>
+      </c>
+      <c r="I158">
+        <v>9.6294999999999992E-3</v>
+      </c>
+      <c r="J158">
+        <v>0.79915610000000004</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>32</v>
+      </c>
+      <c r="B159">
+        <v>80</v>
+      </c>
+      <c r="C159">
+        <v>80</v>
+      </c>
+      <c r="D159">
+        <v>819</v>
+      </c>
+      <c r="E159">
+        <v>114.6152871</v>
+      </c>
+      <c r="F159">
+        <v>1.5366096</v>
+      </c>
+      <c r="G159">
+        <v>112.7973214</v>
+      </c>
+      <c r="H159" t="s">
+        <v>190</v>
+      </c>
+      <c r="I159" s="1">
+        <v>8.1299999999999997E-5</v>
+      </c>
+      <c r="J159">
+        <v>4.4783000000000003E-2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>30</v>
+      </c>
+      <c r="B160">
+        <v>57</v>
+      </c>
+      <c r="C160">
+        <v>60</v>
+      </c>
+      <c r="D160">
+        <v>120</v>
+      </c>
+      <c r="E160">
+        <v>3.0069802999999999</v>
+      </c>
+      <c r="F160">
+        <v>0.71542609999999995</v>
+      </c>
+      <c r="G160">
+        <v>2.1427691000000002</v>
+      </c>
+      <c r="H160" t="s">
+        <v>191</v>
+      </c>
+      <c r="I160" s="1">
+        <v>3.6100000000000003E-5</v>
+      </c>
+      <c r="J160">
+        <v>2.6470799999999999E-2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>28</v>
+      </c>
+      <c r="B161">
+        <v>71</v>
+      </c>
+      <c r="C161">
+        <v>130</v>
+      </c>
+      <c r="D161">
+        <v>127</v>
+      </c>
+      <c r="E161">
+        <v>2.7836987</v>
+      </c>
+      <c r="F161">
+        <v>0.93154700000000001</v>
+      </c>
+      <c r="G161">
+        <v>1.5634424</v>
+      </c>
+      <c r="H161" t="s">
+        <v>192</v>
+      </c>
+      <c r="I161" s="1">
+        <v>3.01E-5</v>
+      </c>
+      <c r="J161">
+        <v>1.54173E-2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>25</v>
+      </c>
+      <c r="B162">
+        <v>93</v>
+      </c>
+      <c r="C162">
+        <v>517</v>
+      </c>
+      <c r="D162">
+        <v>384</v>
+      </c>
+      <c r="E162">
+        <v>61.381271400000003</v>
+      </c>
+      <c r="F162">
+        <v>2.4432079</v>
+      </c>
+      <c r="G162">
+        <v>56.992885200000003</v>
+      </c>
+      <c r="H162" t="s">
+        <v>193</v>
+      </c>
+      <c r="I162" s="1">
+        <v>8.4300000000000003E-5</v>
+      </c>
+      <c r="J162">
+        <v>5.4932300000000003E-2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>22</v>
+      </c>
+      <c r="B163">
+        <v>42</v>
+      </c>
+      <c r="C163">
+        <v>300</v>
+      </c>
+      <c r="D163">
+        <v>300</v>
+      </c>
+      <c r="E163">
+        <v>37.739881799999999</v>
+      </c>
+      <c r="F163">
+        <v>2.3379588</v>
+      </c>
+      <c r="G163">
+        <v>33.173697799999999</v>
+      </c>
+      <c r="H163" t="s">
+        <v>194</v>
+      </c>
+      <c r="I163" s="1">
+        <v>6.7999999999999999E-5</v>
+      </c>
+      <c r="J163">
+        <v>2.6343700000000001E-2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>19</v>
+      </c>
+      <c r="B164">
+        <v>42</v>
+      </c>
+      <c r="C164">
+        <v>81</v>
+      </c>
+      <c r="D164">
+        <v>81</v>
+      </c>
+      <c r="E164">
+        <v>4.2653983000000002</v>
+      </c>
+      <c r="F164">
+        <v>0.50970990000000005</v>
+      </c>
+      <c r="G164">
+        <v>2.8909935</v>
+      </c>
+      <c r="H164" t="s">
+        <v>195</v>
+      </c>
+      <c r="I164" s="1">
+        <v>3.0700000000000001E-5</v>
+      </c>
+      <c r="J164">
+        <v>2.3063400000000001E-2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>17</v>
+      </c>
+      <c r="B165">
+        <v>3</v>
+      </c>
+      <c r="C165">
+        <v>39</v>
+      </c>
+      <c r="D165">
+        <v>39</v>
+      </c>
+      <c r="E165">
+        <v>3.1530344000000001</v>
+      </c>
+      <c r="F165">
+        <v>0.20612929999999999</v>
+      </c>
+      <c r="G165">
+        <v>1.6446372</v>
+      </c>
+      <c r="H165" t="s">
+        <v>196</v>
+      </c>
+      <c r="I165" s="1">
+        <v>2.7100000000000001E-5</v>
+      </c>
+      <c r="J165">
+        <v>3.4385499999999999E-2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>13</v>
+      </c>
+      <c r="B166">
+        <v>22</v>
+      </c>
+      <c r="C166">
+        <v>146</v>
+      </c>
+      <c r="D166">
+        <v>144</v>
+      </c>
+      <c r="E166">
+        <v>5.2921792999999999</v>
+      </c>
+      <c r="F166">
+        <v>0.50159699999999996</v>
+      </c>
+      <c r="G166">
+        <v>3.2439770000000001</v>
+      </c>
+      <c r="H166" t="s">
+        <v>197</v>
+      </c>
+      <c r="I166" s="1">
+        <v>3.0700000000000001E-5</v>
+      </c>
+      <c r="J166" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>15</v>
+      </c>
+      <c r="B167">
+        <v>125</v>
+      </c>
+      <c r="C167">
+        <v>92</v>
+      </c>
+      <c r="D167">
+        <v>30</v>
+      </c>
+      <c r="E167">
+        <v>2.6095185000000001</v>
+      </c>
+      <c r="F167">
+        <v>1.1105868999999999</v>
+      </c>
+      <c r="G167">
+        <v>1.2486288999999999</v>
+      </c>
+      <c r="H167" t="s">
+        <v>198</v>
+      </c>
+      <c r="I167" s="1">
+        <v>3.43E-5</v>
+      </c>
+      <c r="J167" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>